<commit_message>
Gantt Chart V 3
</commit_message>
<xml_diff>
--- a/GOAES.xlsx
+++ b/GOAES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/512f0b414f2a6f27/Data Analytics U3/SAT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC1048D6A91B4A5E5ADE58E9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3050F0CD-F9AB-40CA-9BAF-6F27881507E6}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_F25DC773A252ABDACC1048D6A91B4A5E5ADE58E9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D1B1663B-8413-4C2F-85E6-33AB22A2D90D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC398624-6150-4C7C-9852-B4072C916146}">
   <dimension ref="A1:D364"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5826,8 +5826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D99C0B-B789-4177-B763-ED86E4CC4A59}">
   <dimension ref="A1:N160"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B1048365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12887,6 +12887,15 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048365" xr:uid="{CCA443A6-E5DE-42B9-A418-66379F276152}">
+      <formula1>0</formula1>
+      <formula2>400</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048365" xr:uid="{506B1D8C-E0CF-4446-B63C-049E3F6258B0}">
+      <formula1>"""Yes"",""No"""</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -12899,16 +12908,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FF03D1-A727-4997-9922-7AAA53B375CA}">
   <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -15782,6 +15791,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048410" xr:uid="{229068A6-D837-4006-980D-BDF39385A8C3}">
+      <formula1>1</formula1>
+      <formula2>400</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>